<commit_message>
Updated Viki excel file
</commit_message>
<xml_diff>
--- a/Viki Audio Link extractor & Merger.xlsx
+++ b/Viki Audio Link extractor & Merger.xlsx
@@ -16,42 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>C:\Program Files (x86)\Internet Download Manager\idman.exe</t>
   </si>
   <si>
     <t>/a /d "</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174424v/dash/1174424v_dash_high_360p_3eef59_2012180544_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174425v/dash/1174425v_dash_high_360p_9e93e4_2012180547_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174426v/dash/1174426v_dash_high_360p_97dcac_2012191453_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174427v/dash/1174427v_dash_high_360p_a747dd_2012201504_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174428v/dash/1174428v_dash_high_360p_202712_2012261433_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174429v/dash/1174429v_dash_high_360p_cd35fb_2012271515_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174430v/dash/1174430v_dash_high_360p_01ef16_2101021555_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174431v/dash/1174431v_dash_high_360p_5c5408_2101031429_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174432v/dash/1174432v_dash_high_360p_4ea24c_2101091509_track1_dashinit.mp4</t>
-  </si>
-  <si>
-    <t>https://vikidash-4.akamaized.net/1174433v/dash/1174433v_dash_high_360p_2ced9f_2101101501_track1_dashinit.mp4</t>
   </si>
   <si>
     <t>Index</t>
@@ -64,9 +34,6 @@
   </si>
   <si>
     <t xml:space="preserve">" /f </t>
-  </si>
-  <si>
-    <t>C:\Users\gmastergreatee\Downloads\Video\Mr. Queen</t>
   </si>
   <si>
     <t>Video Count</t>
@@ -108,25 +75,16 @@
     <t>Destination Directory</t>
   </si>
   <si>
-    <t>C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target</t>
-  </si>
-  <si>
     <t>Batch Commands</t>
   </si>
   <si>
     <t>URL(Enter URLs below from Youtube-DL GUI)</t>
   </si>
   <si>
-    <t>Batch Commands(Copy these &amp; run in CMD)</t>
-  </si>
-  <si>
     <t>Make sure mp4, mp3 &amp; srt files are all here</t>
   </si>
   <si>
     <t>eng</t>
-  </si>
-  <si>
-    <t>jpn</t>
   </si>
   <si>
     <t>Video Start</t>
@@ -148,6 +106,30 @@
   </si>
   <si>
     <t>/d = download link or url</t>
+  </si>
+  <si>
+    <t>kor</t>
+  </si>
+  <si>
+    <t>https://vikidash-4.akamaized.net/1174436v/dash/1174436v_dash_high_360p_c36817_2101231458_track1_dashinit.mp4</t>
+  </si>
+  <si>
+    <t>https://vikidash-4.akamaized.net/1174437v/dash/1174437v_dash_high_360p_a72443_2101241445_track1_dashinit.mp4</t>
+  </si>
+  <si>
+    <t>C:\Users\gmastergreatee\Downloads\RAW</t>
+  </si>
+  <si>
+    <t>C:\Users\gmastergreatee\Downloads\RAW\Target</t>
+  </si>
+  <si>
+    <t>Video Number</t>
+  </si>
+  <si>
+    <t>Batch Commands(Copy these, create BAT file &amp; run)</t>
+  </si>
+  <si>
+    <t>Video Counter Start (First Episode Number - generally 1 unless you are downloading a particular episode)</t>
   </si>
 </sst>
 </file>
@@ -322,7 +304,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -371,6 +353,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="5" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -671,24 +656,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J203"/>
+  <dimension ref="A1:J205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="45.42578125" customWidth="1"/>
+    <col min="1" max="1" width="108.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="17" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -696,234 +681,185 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="16" t="s">
+      <c r="A4" s="23">
         <v>13</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="str">
-        <f>IF(LEN(TRIM('IDM Codes'!A5))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A5, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B5,"00"), ". Episode_", TEXT('IDM Codes'!B5,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174424v/dash/1174424v_dash_high_360p_3eef59_2012180544_track1_dashinit.mp4" /f "01. Episode_01.mp4"</v>
-      </c>
-      <c r="D5" s="3" t="str">
-        <f>IF(LEN(TRIM('IDM Codes'!A5))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A5, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B5, "00"),". Episode_", TEXT('IDM Codes'!B5, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174424v/dash/1174424v_dash_high_360p_3eef59_2012180544_track2_dashinit.mp4" /f "01. Episode_01.mp3"</v>
-      </c>
-      <c r="E5" s="3" t="str">
-        <f>IF(LEN(TRIM('IDM Codes'!A5))=0, "", C5&amp;" &amp; "&amp;D5)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174424v/dash/1174424v_dash_high_360p_3eef59_2012180544_track1_dashinit.mp4" /f "01. Episode_01.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174424v/dash/1174424v_dash_high_360p_3eef59_2012180544_track2_dashinit.mp4" /f "01. Episode_01.mp3"</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <f>IF(LEN(TRIM('IDM Codes'!A6))=0,"", INT('IDM Codes'!B5)+1)</f>
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="str">
-        <f>IF(LEN(TRIM('IDM Codes'!A6))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A6, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B6,"00"), ". Episode_", TEXT('IDM Codes'!B6,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174425v/dash/1174425v_dash_high_360p_9e93e4_2012180547_track1_dashinit.mp4" /f "02. Episode_02.mp4"</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>IF(LEN(TRIM('IDM Codes'!A6))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A6, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B6, "00"),". Episode_", TEXT('IDM Codes'!B6, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174425v/dash/1174425v_dash_high_360p_9e93e4_2012180547_track2_dashinit.mp4" /f "02. Episode_02.mp3"</v>
-      </c>
-      <c r="E6" s="3" t="str">
-        <f>IF(LEN(TRIM('IDM Codes'!A6))=0, "", C6&amp;" &amp; "&amp;D6)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174425v/dash/1174425v_dash_high_360p_9e93e4_2012180547_track1_dashinit.mp4" /f "02. Episode_02.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174425v/dash/1174425v_dash_high_360p_9e93e4_2012180547_track2_dashinit.mp4" /f "02. Episode_02.mp3"</v>
+      <c r="D6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B7">
-        <f>IF(LEN(TRIM('IDM Codes'!A7))=0,"", INT('IDM Codes'!B6)+1)</f>
-        <v>3</v>
+        <f>A4</f>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A7))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A7, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B7,"00"), ". Episode_", TEXT('IDM Codes'!B7,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174426v/dash/1174426v_dash_high_360p_97dcac_2012191453_track1_dashinit.mp4" /f "03. Episode_03.mp4"</v>
+        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174436v/dash/1174436v_dash_high_360p_c36817_2101231458_track1_dashinit.mp4" /f "13. Episode_13.mp4"</v>
       </c>
       <c r="D7" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A7))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A7, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B7, "00"),". Episode_", TEXT('IDM Codes'!B7, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174426v/dash/1174426v_dash_high_360p_97dcac_2012191453_track2_dashinit.mp4" /f "03. Episode_03.mp3"</v>
+        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174436v/dash/1174436v_dash_high_360p_c36817_2101231458_track2_dashinit.mp4" /f "13. Episode_13.mp3"</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A7))=0, "", C7&amp;" &amp; "&amp;D7)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174426v/dash/1174426v_dash_high_360p_97dcac_2012191453_track1_dashinit.mp4" /f "03. Episode_03.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174426v/dash/1174426v_dash_high_360p_97dcac_2012191453_track2_dashinit.mp4" /f "03. Episode_03.mp3"</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174436v/dash/1174436v_dash_high_360p_c36817_2101231458_track1_dashinit.mp4" /f "13. Episode_13.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174436v/dash/1174436v_dash_high_360p_c36817_2101231458_track2_dashinit.mp4" /f "13. Episode_13.mp3"</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <f>IF(LEN(TRIM('IDM Codes'!A8))=0,"", INT('IDM Codes'!B7)+1)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A8))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A8, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B8,"00"), ". Episode_", TEXT('IDM Codes'!B8,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174427v/dash/1174427v_dash_high_360p_a747dd_2012201504_track1_dashinit.mp4" /f "04. Episode_04.mp4"</v>
+        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174437v/dash/1174437v_dash_high_360p_a72443_2101241445_track1_dashinit.mp4" /f "14. Episode_14.mp4"</v>
       </c>
       <c r="D8" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A8))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A8, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B8, "00"),". Episode_", TEXT('IDM Codes'!B8, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174427v/dash/1174427v_dash_high_360p_a747dd_2012201504_track2_dashinit.mp4" /f "04. Episode_04.mp3"</v>
+        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174437v/dash/1174437v_dash_high_360p_a72443_2101241445_track2_dashinit.mp4" /f "14. Episode_14.mp3"</v>
       </c>
       <c r="E8" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A8))=0, "", C8&amp;" &amp; "&amp;D8)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174427v/dash/1174427v_dash_high_360p_a747dd_2012201504_track1_dashinit.mp4" /f "04. Episode_04.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174427v/dash/1174427v_dash_high_360p_a747dd_2012201504_track2_dashinit.mp4" /f "04. Episode_04.mp3"</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174437v/dash/1174437v_dash_high_360p_a72443_2101241445_track1_dashinit.mp4" /f "14. Episode_14.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174437v/dash/1174437v_dash_high_360p_a72443_2101241445_track2_dashinit.mp4" /f "14. Episode_14.mp3"</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
+      <c r="B9" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A9))=0,"", INT('IDM Codes'!B8)+1)</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="C9" s="2" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A9))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A9, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B9,"00"), ". Episode_", TEXT('IDM Codes'!B9,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174428v/dash/1174428v_dash_high_360p_202712_2012261433_track1_dashinit.mp4" /f "05. Episode_05.mp4"</v>
+        <v/>
       </c>
       <c r="D9" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A9))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A9, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B9, "00"),". Episode_", TEXT('IDM Codes'!B9, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174428v/dash/1174428v_dash_high_360p_202712_2012261433_track2_dashinit.mp4" /f "05. Episode_05.mp3"</v>
+        <v/>
       </c>
       <c r="E9" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A9))=0, "", C9&amp;" &amp; "&amp;D9)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174428v/dash/1174428v_dash_high_360p_202712_2012261433_track1_dashinit.mp4" /f "05. Episode_05.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174428v/dash/1174428v_dash_high_360p_202712_2012261433_track2_dashinit.mp4" /f "05. Episode_05.mp3"</v>
-      </c>
+        <v/>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
+      <c r="B10" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A10))=0,"", INT('IDM Codes'!B9)+1)</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="C10" s="2" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A10))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A10, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B10,"00"), ". Episode_", TEXT('IDM Codes'!B10,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174429v/dash/1174429v_dash_high_360p_cd35fb_2012271515_track1_dashinit.mp4" /f "06. Episode_06.mp4"</v>
+        <v/>
       </c>
       <c r="D10" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A10))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A10, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B10, "00"),". Episode_", TEXT('IDM Codes'!B10, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174429v/dash/1174429v_dash_high_360p_cd35fb_2012271515_track2_dashinit.mp4" /f "06. Episode_06.mp3"</v>
+        <v/>
       </c>
       <c r="E10" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A10))=0, "", C10&amp;" &amp; "&amp;D10)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174429v/dash/1174429v_dash_high_360p_cd35fb_2012271515_track1_dashinit.mp4" /f "06. Episode_06.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174429v/dash/1174429v_dash_high_360p_cd35fb_2012271515_track2_dashinit.mp4" /f "06. Episode_06.mp3"</v>
-      </c>
+        <v/>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
+      <c r="B11" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A11))=0,"", INT('IDM Codes'!B10)+1)</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="C11" s="2" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A11))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A11, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B11,"00"), ". Episode_", TEXT('IDM Codes'!B11,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174430v/dash/1174430v_dash_high_360p_01ef16_2101021555_track1_dashinit.mp4" /f "07. Episode_07.mp4"</v>
+        <v/>
       </c>
       <c r="D11" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A11))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A11, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B11, "00"),". Episode_", TEXT('IDM Codes'!B11, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174430v/dash/1174430v_dash_high_360p_01ef16_2101021555_track2_dashinit.mp4" /f "07. Episode_07.mp3"</v>
+        <v/>
       </c>
       <c r="E11" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A11))=0, "", C11&amp;" &amp; "&amp;D11)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174430v/dash/1174430v_dash_high_360p_01ef16_2101021555_track1_dashinit.mp4" /f "07. Episode_07.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174430v/dash/1174430v_dash_high_360p_01ef16_2101021555_track2_dashinit.mp4" /f "07. Episode_07.mp3"</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
+      <c r="B12" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A12))=0,"", INT('IDM Codes'!B11)+1)</f>
-        <v>8</v>
+        <v/>
       </c>
       <c r="C12" s="2" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A12))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A12, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B12,"00"), ". Episode_", TEXT('IDM Codes'!B12,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174431v/dash/1174431v_dash_high_360p_5c5408_2101031429_track1_dashinit.mp4" /f "08. Episode_08.mp4"</v>
+        <v/>
       </c>
       <c r="D12" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A12))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A12, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B12, "00"),". Episode_", TEXT('IDM Codes'!B12, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174431v/dash/1174431v_dash_high_360p_5c5408_2101031429_track2_dashinit.mp4" /f "08. Episode_08.mp3"</v>
+        <v/>
       </c>
       <c r="E12" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A12))=0, "", C12&amp;" &amp; "&amp;D12)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174431v/dash/1174431v_dash_high_360p_5c5408_2101031429_track1_dashinit.mp4" /f "08. Episode_08.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174431v/dash/1174431v_dash_high_360p_5c5408_2101031429_track2_dashinit.mp4" /f "08. Episode_08.mp3"</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
+      <c r="B13" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A13))=0,"", INT('IDM Codes'!B12)+1)</f>
-        <v>9</v>
+        <v/>
       </c>
       <c r="C13" s="2" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A13))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A13, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B13,"00"), ". Episode_", TEXT('IDM Codes'!B13,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174432v/dash/1174432v_dash_high_360p_4ea24c_2101091509_track1_dashinit.mp4" /f "09. Episode_09.mp4"</v>
+        <v/>
       </c>
       <c r="D13" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A13))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A13, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B13, "00"),". Episode_", TEXT('IDM Codes'!B13, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174432v/dash/1174432v_dash_high_360p_4ea24c_2101091509_track2_dashinit.mp4" /f "09. Episode_09.mp3"</v>
+        <v/>
       </c>
       <c r="E13" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A13))=0, "", C13&amp;" &amp; "&amp;D13)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174432v/dash/1174432v_dash_high_360p_4ea24c_2101091509_track1_dashinit.mp4" /f "09. Episode_09.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174432v/dash/1174432v_dash_high_360p_4ea24c_2101091509_track2_dashinit.mp4" /f "09. Episode_09.mp3"</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
+      <c r="B14" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A14))=0,"", INT('IDM Codes'!B13)+1)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="C14" s="2" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A14))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A14, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B14,"00"), ". Episode_", TEXT('IDM Codes'!B14,"00"), ".mp4"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174433v/dash/1174433v_dash_high_360p_2ced9f_2101101501_track1_dashinit.mp4" /f "10. Episode_10.mp4"</v>
+        <v/>
       </c>
       <c r="D14" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A14))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A14, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B14, "00"),". Episode_", TEXT('IDM Codes'!B14, "00"), ".mp3"""))</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174433v/dash/1174433v_dash_high_360p_2ced9f_2101101501_track2_dashinit.mp4" /f "10. Episode_10.mp3"</v>
+        <v/>
       </c>
       <c r="E14" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A14))=0, "", C14&amp;" &amp; "&amp;D14)</f>
-        <v>"C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174433v/dash/1174433v_dash_high_360p_2ced9f_2101101501_track1_dashinit.mp4" /f "10. Episode_10.mp4" &amp; "C:\Program Files (x86)\Internet Download Manager\idman.exe" /a /d "https://vikidash-4.akamaized.net/1174433v/dash/1174433v_dash_high_360p_2ced9f_2101101501_track2_dashinit.mp4" /f "10. Episode_10.mp3"</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -4316,7 +4252,7 @@
         <v/>
       </c>
       <c r="C203" s="2" t="str">
-        <f>IF(LEN(TRIM('IDM Codes'!A203))=0, "", CONCATENATE("""", 'IDM Params'!#REF!, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A203, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B203,"00"), ". Episode_", TEXT('IDM Codes'!B203,"00"), ".mp4"""))</f>
+        <f>IF(LEN(TRIM('IDM Codes'!A203))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A203, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B203,"00"), ". Episode_", TEXT('IDM Codes'!B203,"00"), ".mp4"""))</f>
         <v/>
       </c>
       <c r="D203" s="3" t="str">
@@ -4325,6 +4261,42 @@
       </c>
       <c r="E203" s="3" t="str">
         <f>IF(LEN(TRIM('IDM Codes'!A203))=0, "", C203&amp;" &amp; "&amp;D203)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="204" spans="2:5">
+      <c r="B204" t="str">
+        <f>IF(LEN(TRIM('IDM Codes'!A204))=0,"", INT('IDM Codes'!B203)+1)</f>
+        <v/>
+      </c>
+      <c r="C204" s="2" t="str">
+        <f>IF(LEN(TRIM('IDM Codes'!A204))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A204, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B204,"00"), ". Episode_", TEXT('IDM Codes'!B204,"00"), ".mp4"""))</f>
+        <v/>
+      </c>
+      <c r="D204" s="3" t="str">
+        <f>IF(LEN(TRIM('IDM Codes'!A204))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A204, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B204, "00"),". Episode_", TEXT('IDM Codes'!B204, "00"), ".mp3"""))</f>
+        <v/>
+      </c>
+      <c r="E204" s="3" t="str">
+        <f>IF(LEN(TRIM('IDM Codes'!A204))=0, "", C204&amp;" &amp; "&amp;D204)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="205" spans="2:5">
+      <c r="B205" t="str">
+        <f>IF(LEN(TRIM('IDM Codes'!A205))=0,"", INT('IDM Codes'!B204)+1)</f>
+        <v/>
+      </c>
+      <c r="C205" s="2" t="str">
+        <f>IF(LEN(TRIM('IDM Codes'!A205))=0, "", CONCATENATE("""", 'IDM Params'!#REF!, """", " ", 'IDM Params'!$A$1,'IDM Codes'!A205, 'IDM Params'!$A$2,"""", TEXT('IDM Codes'!B205,"00"), ". Episode_", TEXT('IDM Codes'!B205,"00"), ".mp4"""))</f>
+        <v/>
+      </c>
+      <c r="D205" s="3" t="str">
+        <f>IF(LEN(TRIM('IDM Codes'!A205))=0, "", CONCATENATE("""", 'IDM Codes'!$A$2,""""," ",'IDM Params'!$A$1,SUBSTITUTE('IDM Codes'!A205, "track1","track2"), 'IDM Params'!$A$2,"""",  TEXT('IDM Codes'!B205, "00"),". Episode_", TEXT('IDM Codes'!B205, "00"), ".mp3"""))</f>
+        <v/>
+      </c>
+      <c r="E205" s="3" t="str">
+        <f>IF(LEN(TRIM('IDM Codes'!A205))=0, "", C205&amp;" &amp; "&amp;D205)</f>
         <v/>
       </c>
     </row>
@@ -4339,7 +4311,7 @@
   <dimension ref="A1:K201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="B14" sqref="B14:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4353,21 +4325,21 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -4376,18 +4348,18 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B4" s="14">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F4" s="19" t="str">
         <f>IF(ffmpegCodes!$B$7 = 1, "Dummy SRT file-name (Make sure files are named like this)","")</f>
@@ -4401,14 +4373,14 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B5" s="14">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F5" s="21" t="str">
         <f>IF(ffmpegCodes!$B$7 = 1, TEXT(ffmpegCodes!$B$5, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!$B$5, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt", "")</f>
-        <v>01. Mr. Queen - Episode 1.en.srt</v>
+        <v>13. Mr. Queen - Episode 13.en.srt</v>
       </c>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
@@ -4418,13 +4390,13 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F6" s="22" t="str">
         <f>IF(ffmpegCodes!$B$7 = 1, "To download subtitles, just check the ""Custom Args"" option in ""Youtube-DL GUI"", set the ""Link"" &amp; press ""Get Data"" button. This will download all subtitles to the ""youtube-dl gui"" folder.", "")</f>
@@ -4438,7 +4410,7 @@
     </row>
     <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B7" s="14">
         <v>1</v>
@@ -4452,11 +4424,11 @@
     </row>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B8" s="12" t="str">
         <f>RIGHT(ffmpegCodes!B2,LEN(ffmpegCodes!B2)-SEARCH("/", SUBSTITUTE(ffmpegCodes!B2,"\","/",LEN(ffmpegCodes!B2)-LEN(SUBSTITUTE(ffmpegCodes!B2,"\","")))))</f>
-        <v>Mr. Queen</v>
+        <v>RAW</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
@@ -4467,10 +4439,10 @@
     </row>
     <row r="9" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
@@ -4481,24 +4453,24 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" thickTop="1">
       <c r="A10" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>38</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
@@ -4520,10 +4492,10 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="20"/>
@@ -4537,11 +4509,11 @@
     <row r="14" spans="1:11" ht="15" customHeight="1">
       <c r="A14">
         <f>B5</f>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B14" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A14), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A14, "00"), ". Episode_", TEXT(ffmpegCodes!A14, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A14, "00"), ". Episode_", TEXT(ffmpegCodes!A14, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A14, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A14, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A14, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A14, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\01. Episode_01.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\01. Episode_01.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\01. Mr. Queen - Episode 1.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\01. Episode 01.mp4"</v>
+        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\RAW\13. Episode_13.mp4" -i "C:\Users\gmastergreatee\Downloads\RAW\13. Episode_13.mp3" -i "C:\Users\gmastergreatee\Downloads\RAW\13. Mr. Queen - Episode 13.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="kor" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\RAW\Target\13. Episode 13.mp4"</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="20"/>
@@ -4555,11 +4527,11 @@
     <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="A15">
         <f>IF(ffmpegCodes!A14 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A14 + 1, "")</f>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B15" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A15), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A15, "00"), ". Episode_", TEXT(ffmpegCodes!A15, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A15, "00"), ". Episode_", TEXT(ffmpegCodes!A15, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A15, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A15, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A15, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A15, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\02. Episode_02.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\02. Episode_02.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\02. Mr. Queen - Episode 2.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\02. Episode 02.mp4"</v>
+        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\RAW\14. Episode_14.mp4" -i "C:\Users\gmastergreatee\Downloads\RAW\14. Episode_14.mp3" -i "C:\Users\gmastergreatee\Downloads\RAW\14. Mr. Queen - Episode 14.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="kor" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\RAW\Target\14. Episode 14.mp4"</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="20"/>
@@ -4573,11 +4545,11 @@
     <row r="16" spans="1:11" ht="15" customHeight="1">
       <c r="A16">
         <f>IF(ffmpegCodes!A15 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A15 + 1, "")</f>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B16" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A16), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A16, "00"), ". Episode_", TEXT(ffmpegCodes!A16, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A16, "00"), ". Episode_", TEXT(ffmpegCodes!A16, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A16, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A16, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A16, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A16, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\03. Episode_03.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\03. Episode_03.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\03. Mr. Queen - Episode 3.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\03. Episode 03.mp4"</v>
+        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\RAW\15. Episode_15.mp4" -i "C:\Users\gmastergreatee\Downloads\RAW\15. Episode_15.mp3" -i "C:\Users\gmastergreatee\Downloads\RAW\15. Mr. Queen - Episode 15.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="kor" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\RAW\Target\15. Episode 15.mp4"</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="20"/>
@@ -4589,13 +4561,13 @@
       <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17">
+      <c r="A17" t="str">
         <f>IF(ffmpegCodes!A16 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A16 + 1, "")</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="B17" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A17), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A17, "00"), ". Episode_", TEXT(ffmpegCodes!A17, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A17, "00"), ". Episode_", TEXT(ffmpegCodes!A17, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A17, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A17, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A17, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A17, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\04. Episode_04.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\04. Episode_04.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\04. Mr. Queen - Episode 4.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\04. Episode 04.mp4"</v>
+        <v/>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
@@ -4606,13 +4578,13 @@
       <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
-      <c r="A18">
+      <c r="A18" t="str">
         <f>IF(ffmpegCodes!A17 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A17 + 1, "")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="B18" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A18), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A18, "00"), ". Episode_", TEXT(ffmpegCodes!A18, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A18, "00"), ". Episode_", TEXT(ffmpegCodes!A18, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A18, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A18, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A18, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A18, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\05. Episode_05.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\05. Episode_05.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\05. Mr. Queen - Episode 5.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\05. Episode 05.mp4"</v>
+        <v/>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -4623,13 +4595,13 @@
       <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1">
-      <c r="A19">
+      <c r="A19" t="str">
         <f>IF(ffmpegCodes!A18 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A18 + 1, "")</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="B19" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A19), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A19, "00"), ". Episode_", TEXT(ffmpegCodes!A19, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A19, "00"), ". Episode_", TEXT(ffmpegCodes!A19, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A19, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A19, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A19, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A19, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\06. Episode_06.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\06. Episode_06.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\06. Mr. Queen - Episode 6.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\06. Episode 06.mp4"</v>
+        <v/>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -4640,13 +4612,13 @@
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1">
-      <c r="A20">
+      <c r="A20" t="str">
         <f>IF(ffmpegCodes!A19 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A19 + 1, "")</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="B20" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A20), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A20, "00"), ". Episode_", TEXT(ffmpegCodes!A20, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A20, "00"), ". Episode_", TEXT(ffmpegCodes!A20, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A20, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A20, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A20, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A20, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\07. Episode_07.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\07. Episode_07.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\07. Mr. Queen - Episode 7.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\07. Episode 07.mp4"</v>
+        <v/>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -4657,13 +4629,13 @@
       <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21">
+      <c r="A21" t="str">
         <f>IF(ffmpegCodes!A20 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A20 + 1, "")</f>
-        <v>8</v>
+        <v/>
       </c>
       <c r="B21" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A21), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A21, "00"), ". Episode_", TEXT(ffmpegCodes!A21, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A21, "00"), ". Episode_", TEXT(ffmpegCodes!A21, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A21, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A21, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A21, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A21, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\08. Episode_08.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\08. Episode_08.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\08. Mr. Queen - Episode 8.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\08. Episode 08.mp4"</v>
+        <v/>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -4674,13 +4646,13 @@
       <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22">
+      <c r="A22" t="str">
         <f>IF(ffmpegCodes!A21 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A21 + 1, "")</f>
-        <v>9</v>
+        <v/>
       </c>
       <c r="B22" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A22), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A22, "00"), ". Episode_", TEXT(ffmpegCodes!A22, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A22, "00"), ". Episode_", TEXT(ffmpegCodes!A22, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A22, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A22, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A22, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A22, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\09. Episode_09.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\09. Episode_09.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\09. Mr. Queen - Episode 9.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\09. Episode 09.mp4"</v>
+        <v/>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -4691,23 +4663,23 @@
       <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23">
+      <c r="A23" t="str">
         <f>IF(ffmpegCodes!A22 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A22 + 1, "")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="B23" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A23), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A23, "00"), ". Episode_", TEXT(ffmpegCodes!A23, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A23, "00"), ". Episode_", TEXT(ffmpegCodes!A23, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A23, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A23, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A23, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A23, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\10. Episode_10.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\10. Episode_10.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\10. Mr. Queen - Episode 10.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\10. Episode 10.mp4"</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24">
+      <c r="A24" t="str">
         <f>IF(ffmpegCodes!A23 &lt; ffmpegCodes!$B$4 + ffmpegCodes!$B$5, ffmpegCodes!A23 + 1, "")</f>
-        <v>11</v>
+        <v/>
       </c>
       <c r="B24" s="15" t="str">
         <f>IF(ISNUMBER(ffmpegCodes!A24), CONCATENATE("""",ffmpegCodes!$B$1, "\ffmpeg.exe","""", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A24, "00"), ". Episode_", TEXT(ffmpegCodes!A24, "00"), ".mp4", """", " -i ", """", ffmpegCodes!$B$2, "\", TEXT(ffmpegCodes!A24, "00"), ". Episode_", TEXT(ffmpegCodes!A24, "00"), ".mp3", """")&amp;IF(ffmpegCodes!$B$7 = 0, "", " -i "&amp;""""&amp;ffmpegCodes!$B$2&amp;"\"&amp;TEXT(ffmpegCodes!A24, "00")&amp;". "&amp;ffmpegCodes!$B$9&amp;" - Episode "&amp;TEXT(ffmpegCodes!A24, "0")&amp;"."&amp;ffmpegCodes!$B$11&amp;".srt"&amp;"""")&amp;" -map 0:0 -map 1:0"&amp;IF(ffmpegCodes!$B$7=0,""," -map 2:0")&amp;" -c:v copy -c:a copy"&amp;IF(ffmpegCodes!$B$7=0,""," -c:s mov_text")&amp;" -disposition:s default -metadata:s:a language="""&amp;ffmpegCodes!$B$6&amp;""""&amp;IF(ffmpegCodes!$B$7=0,""," -metadata:s:s language="""&amp;ffmpegCodes!$B$10&amp;"""")&amp;" -y"&amp;" """&amp;ffmpegCodes!$B$3&amp;"\"&amp;TEXT(ffmpegCodes!A24, "00")&amp;". Episode "&amp;TEXT(ffmpegCodes!A24, "00")&amp;".mp4""","")</f>
-        <v>"H:\Softwares\Multimedia\ffmpeg-20170921\ffmpeg.exe" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\11. Episode_11.mp4" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\11. Episode_11.mp3" -i "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\11. Mr. Queen - Episode 11.en.srt" -map 0:0 -map 1:0 -map 2:0 -c:v copy -c:a copy -c:s mov_text -disposition:s default -metadata:s:a language="jpn" -metadata:s:s language="eng" -y "C:\Users\gmastergreatee\Downloads\Video\Mr. Queen\Target\11. Episode 11.mp4"</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -6510,22 +6482,22 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>